<commit_message>
adaptacion a error en ERP por el cual las facturas aunque estaban abonadas con menos del total de la factura, salian como pagas. Esta adaptacion revisa sin importar si esta paga o no, que el monto abonado sea igual al monto total para poder asegurarse de que efectivamente fue pagada.
</commit_message>
<xml_diff>
--- a/excel/debtorsExceptions.xlsx
+++ b/excel/debtorsExceptions.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -413,7 +413,7 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>259</v>
+        <v>388</v>
       </c>
       <c r="B2">
         <v>45925</v>
@@ -436,27 +436,32 @@
     </row>
     <row r="6">
       <c r="A6">
-        <v>2201</v>
+        <v>780</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>388</v>
+        <v>2200</v>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>2200</v>
+        <v>2201</v>
       </c>
     </row>
     <row r="9">
       <c r="A9">
+        <v>2447</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10">
         <v>119</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B10"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:B11"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>